<commit_message>
Vitalparameter aktualisiert, Beispiele separiert
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-t-cabs-communication-atemfrequenz-high-alarm.xlsx
+++ b/output/StructureDefinition-t-cabs-communication-atemfrequenz-high-alarm.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-02T15:35:32+02:00</t>
+    <t>2025-04-11T09:40:45+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -744,7 +744,7 @@
     <t>Communication.about</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://t-cabs.org/StructureDefinition/t-cabs-observation-af)
+    <t xml:space="preserve">Reference(http://t-cabs.org/StructureDefinition/t-cabs-observation-atemfrequenz-beatmet)
 </t>
   </si>
   <si>

</xml_diff>